<commit_message>
Upload document( scan , 화면 디자인 수정 )
</commit_message>
<xml_diff>
--- a/documents/4. diffuser_디자인기획서/04-2_Sitemenu.xlsx
+++ b/documents/4. diffuser_디자인기획서/04-2_Sitemenu.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\문은빈\Documents\카카오톡 받은 파일\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UX410UF\Documents\GitHub\Diffuser\documents\4. diffuser_디자인기획서\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3C784A7-D867-44E1-AD34-ED2FA379446E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F27B4CB4-1B91-475F-81D5-3585B4172315}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-18" yWindow="-18" windowWidth="8610" windowHeight="10560" tabRatio="617" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="617" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="directory" sheetId="11" r:id="rId1"/>
@@ -487,7 +487,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -497,20 +497,15 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -543,7 +538,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -888,38 +882,41 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:H48"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="154" zoomScaleNormal="100" zoomScaleSheetLayoutView="154" workbookViewId="0">
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="11.1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="11.25" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="16.2265625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="15.76953125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="15.31640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="18.54296875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10.453125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="6.54296875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="10.2265625" style="9" customWidth="1"/>
-    <col min="8" max="8" width="34.953125" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="8.86328125" style="1"/>
+    <col min="1" max="1" width="16.21875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="15.77734375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="15.33203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="18.5546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.44140625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="6.5546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="10.21875" style="7" customWidth="1"/>
+    <col min="8" max="8" width="35" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="41.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="26" t="s">
+    <row r="1" spans="1:8" ht="41.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-    </row>
-    <row r="2" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+    </row>
+    <row r="2" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -945,7 +942,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A3" s="3" t="s">
         <v>29</v>
       </c>
@@ -958,229 +955,229 @@
       </c>
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
-      <c r="G3" s="7"/>
+      <c r="G3" s="6"/>
       <c r="H3" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="11.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="12" t="s">
+    <row r="4" spans="1:8" ht="12" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="B4" s="12"/>
-      <c r="C4" s="12"/>
-      <c r="D4" s="12" t="s">
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="E4" s="13" t="s">
+      <c r="E4" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="13"/>
-      <c r="G4" s="14"/>
-      <c r="H4" s="12" t="s">
+      <c r="F4" s="10"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="9" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="11.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="18" t="s">
+    <row r="5" spans="1:8" ht="12" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="18" t="s">
+      <c r="B5" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="18" t="s">
+      <c r="C5" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="D5" s="18" t="s">
+      <c r="D5" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="E5" s="19"/>
-      <c r="F5" s="19"/>
-      <c r="G5" s="20"/>
-      <c r="H5" s="18" t="s">
+      <c r="E5" s="16"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="17"/>
+      <c r="H5" s="15" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="11.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="15" t="s">
+    <row r="6" spans="1:8" ht="12" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="15" t="s">
+      <c r="B6" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="15" t="s">
+      <c r="C6" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="15" t="s">
+      <c r="D6" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="E6" s="16"/>
-      <c r="F6" s="16"/>
-      <c r="G6" s="17"/>
-      <c r="H6" s="15" t="s">
+      <c r="E6" s="13"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="12" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="12.9" x14ac:dyDescent="0.3">
-      <c r="A7" s="15" t="s">
+    <row r="7" spans="1:8" ht="12" x14ac:dyDescent="0.15">
+      <c r="A7" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="B7" s="21" t="s">
+      <c r="B7" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="C7" s="15" t="s">
+      <c r="C7" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="D7" s="15" t="s">
+      <c r="D7" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="E7" s="16"/>
-      <c r="F7" s="16"/>
-      <c r="G7" s="17"/>
-      <c r="H7" s="21" t="s">
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="18" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.15">
       <c r="B8" s="3" t="s">
         <v>35</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="D8" s="11" t="s">
+      <c r="D8" s="8" t="s">
         <v>51</v>
       </c>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
-      <c r="G8" s="7"/>
+      <c r="G8" s="6"/>
       <c r="H8" s="3" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" s="12"/>
-      <c r="B9" s="12" t="s">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A9" s="9"/>
+      <c r="B9" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="C9" s="12" t="s">
+      <c r="C9" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="D9" s="22" t="s">
+      <c r="D9" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="E9" s="13" t="s">
+      <c r="E9" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="F9" s="13"/>
-      <c r="G9" s="14"/>
-      <c r="H9" s="12" t="s">
+      <c r="F9" s="10"/>
+      <c r="G9" s="11"/>
+      <c r="H9" s="9" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="12"/>
-      <c r="B10" s="12" t="s">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A10" s="9"/>
+      <c r="B10" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="C10" s="12" t="s">
+      <c r="C10" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="D10" s="12" t="s">
+      <c r="D10" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="E10" s="13" t="s">
+      <c r="E10" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="F10" s="12"/>
-      <c r="G10" s="12"/>
-      <c r="H10" s="12" t="s">
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" s="12" t="s">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A11" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="B11" s="12" t="s">
+      <c r="B11" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="C11" s="12" t="s">
+      <c r="C11" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="D11" s="22" t="s">
+      <c r="D11" s="19" t="s">
         <v>75</v>
       </c>
-      <c r="E11" s="13" t="s">
+      <c r="E11" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="F11" s="13"/>
-      <c r="G11" s="14"/>
-      <c r="H11" s="12" t="s">
+      <c r="F11" s="10"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="9" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" s="12"/>
-      <c r="B12" s="12" t="s">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A12" s="9"/>
+      <c r="B12" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="C12" s="12" t="s">
+      <c r="C12" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="D12" s="22" t="s">
+      <c r="D12" s="19" t="s">
         <v>74</v>
       </c>
-      <c r="E12" s="13" t="s">
+      <c r="E12" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="F12" s="13"/>
-      <c r="G12" s="14"/>
-      <c r="H12" s="12" t="s">
+      <c r="F12" s="10"/>
+      <c r="G12" s="11"/>
+      <c r="H12" s="9" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="11.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" ht="12" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A13" s="3"/>
-      <c r="B13" s="12" t="s">
+      <c r="B13" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="C13" s="12" t="s">
+      <c r="C13" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="D13" s="22" t="s">
+      <c r="D13" s="19" t="s">
         <v>76</v>
       </c>
-      <c r="E13" s="13" t="s">
+      <c r="E13" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="F13" s="13"/>
-      <c r="G13" s="14"/>
-      <c r="H13" s="12" t="s">
+      <c r="F13" s="10"/>
+      <c r="G13" s="11"/>
+      <c r="H13" s="9" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A14" s="15" t="s">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A14" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="15" t="s">
+      <c r="B14" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="C14" s="15" t="s">
+      <c r="C14" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="D14" s="15" t="s">
+      <c r="D14" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="E14" s="16"/>
-      <c r="F14" s="16"/>
-      <c r="G14" s="17"/>
-      <c r="H14" s="15" t="s">
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="12" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A15" s="3"/>
       <c r="B15" s="3" t="s">
         <v>15</v>
@@ -1188,19 +1185,19 @@
       <c r="C15" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="D15" s="11" t="s">
+      <c r="D15" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="E15" s="23" t="s">
+      <c r="E15" s="20" t="s">
         <v>45</v>
       </c>
       <c r="F15" s="4"/>
-      <c r="G15" s="7"/>
+      <c r="G15" s="6"/>
       <c r="H15" s="3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A16" s="3"/>
       <c r="B16" s="3" t="s">
         <v>16</v>
@@ -1208,370 +1205,205 @@
       <c r="C16" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="D16" s="11" t="s">
+      <c r="D16" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="E16" s="23" t="s">
+      <c r="E16" s="20" t="s">
         <v>45</v>
       </c>
       <c r="F16" s="4"/>
-      <c r="G16" s="7"/>
+      <c r="G16" s="6"/>
       <c r="H16" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="11.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="12"/>
-      <c r="B17" s="12" t="s">
+    <row r="17" spans="1:8" ht="12" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="9"/>
+      <c r="B17" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="C17" s="12" t="s">
+      <c r="C17" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="D17" s="22" t="s">
+      <c r="D17" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="E17" s="24" t="s">
+      <c r="E17" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="F17" s="13"/>
-      <c r="G17" s="14"/>
-      <c r="H17" s="12" t="s">
+      <c r="F17" s="10"/>
+      <c r="G17" s="11"/>
+      <c r="H17" s="9" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A18" s="15" t="s">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A18" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="B18" s="15" t="s">
+      <c r="B18" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="C18" s="15"/>
-      <c r="D18" s="25" t="s">
+      <c r="C18" s="12"/>
+      <c r="D18" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="E18" s="16" t="s">
+      <c r="E18" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="F18" s="16"/>
-      <c r="G18" s="17"/>
-      <c r="H18" s="15" t="s">
+      <c r="F18" s="13"/>
+      <c r="G18" s="14"/>
+      <c r="H18" s="12" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A19" s="3"/>
       <c r="B19" s="3" t="s">
         <v>18</v>
       </c>
       <c r="C19" s="3"/>
-      <c r="D19" s="10" t="s">
+      <c r="D19" s="3" t="s">
         <v>62</v>
       </c>
       <c r="E19" s="4" t="s">
         <v>2</v>
       </c>
       <c r="F19" s="4"/>
-      <c r="G19" s="7"/>
+      <c r="G19" s="6"/>
       <c r="H19" s="3" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A20" s="3"/>
       <c r="B20" s="3" t="s">
         <v>23</v>
       </c>
       <c r="C20" s="3"/>
-      <c r="D20" s="10" t="s">
+      <c r="D20" s="3" t="s">
         <v>61</v>
       </c>
       <c r="E20" s="4" t="s">
         <v>2</v>
       </c>
       <c r="F20" s="4"/>
-      <c r="G20" s="7"/>
+      <c r="G20" s="6"/>
       <c r="H20" s="3" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A21" s="5"/>
-      <c r="B21" s="5"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="6"/>
-      <c r="G21" s="8"/>
-      <c r="H21" s="5"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A22" s="5"/>
-      <c r="B22" s="5"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="6"/>
-      <c r="F22" s="6"/>
-      <c r="G22" s="8"/>
-      <c r="H22" s="5"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A23" s="5"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="6"/>
-      <c r="F23" s="6"/>
-      <c r="G23" s="8"/>
-      <c r="H23" s="5"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A24" s="5"/>
-      <c r="B24" s="5"/>
-      <c r="C24" s="5"/>
-      <c r="D24" s="5"/>
-      <c r="E24" s="6"/>
-      <c r="F24" s="6"/>
-      <c r="G24" s="8"/>
-      <c r="H24" s="5"/>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A25" s="5"/>
-      <c r="B25" s="5"/>
-      <c r="C25" s="5"/>
-      <c r="D25" s="5"/>
-      <c r="E25" s="6"/>
-      <c r="F25" s="6"/>
-      <c r="G25" s="8"/>
-      <c r="H25" s="5"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A26" s="5"/>
-      <c r="B26" s="5"/>
-      <c r="C26" s="5"/>
-      <c r="D26" s="5"/>
-      <c r="E26" s="6"/>
-      <c r="F26" s="6"/>
-      <c r="G26" s="8"/>
-      <c r="H26" s="5"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A27" s="5"/>
-      <c r="B27" s="5"/>
-      <c r="C27" s="5"/>
-      <c r="D27" s="5"/>
-      <c r="E27" s="6"/>
-      <c r="F27" s="6"/>
-      <c r="G27" s="8"/>
-      <c r="H27" s="5"/>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A28" s="5"/>
-      <c r="B28" s="5"/>
-      <c r="C28" s="5"/>
-      <c r="D28" s="5"/>
-      <c r="E28" s="6"/>
-      <c r="F28" s="6"/>
-      <c r="G28" s="8"/>
-      <c r="H28" s="5"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A29" s="5"/>
-      <c r="B29" s="5"/>
-      <c r="C29" s="5"/>
-      <c r="D29" s="5"/>
-      <c r="E29" s="6"/>
-      <c r="F29" s="6"/>
-      <c r="G29" s="8"/>
-      <c r="H29" s="5"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A30" s="5"/>
-      <c r="B30" s="5"/>
-      <c r="C30" s="5"/>
-      <c r="D30" s="5"/>
-      <c r="E30" s="6"/>
-      <c r="F30" s="6"/>
-      <c r="G30" s="8"/>
-      <c r="H30" s="5"/>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A31" s="5"/>
-      <c r="B31" s="5"/>
-      <c r="C31" s="5"/>
-      <c r="D31" s="5"/>
-      <c r="E31" s="6"/>
-      <c r="F31" s="6"/>
-      <c r="G31" s="8"/>
-      <c r="H31" s="5"/>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A32" s="5"/>
-      <c r="B32" s="5"/>
-      <c r="C32" s="5"/>
-      <c r="D32" s="5"/>
-      <c r="E32" s="6"/>
-      <c r="F32" s="6"/>
-      <c r="G32" s="8"/>
-      <c r="H32" s="5"/>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A33" s="5"/>
-      <c r="B33" s="5"/>
-      <c r="C33" s="5"/>
-      <c r="D33" s="5"/>
-      <c r="E33" s="6"/>
-      <c r="F33" s="6"/>
-      <c r="G33" s="8"/>
-      <c r="H33" s="5"/>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A34" s="5"/>
-      <c r="B34" s="5"/>
-      <c r="C34" s="5"/>
-      <c r="D34" s="5"/>
-      <c r="E34" s="6"/>
-      <c r="F34" s="6"/>
-      <c r="G34" s="8"/>
-      <c r="H34" s="5"/>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A35" s="5"/>
-      <c r="B35" s="5"/>
-      <c r="C35" s="5"/>
-      <c r="D35" s="5"/>
-      <c r="E35" s="6"/>
-      <c r="F35" s="6"/>
-      <c r="G35" s="8"/>
-      <c r="H35" s="5"/>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A36" s="5"/>
-      <c r="B36" s="5"/>
-      <c r="C36" s="5"/>
-      <c r="D36" s="5"/>
-      <c r="E36" s="6"/>
-      <c r="F36" s="6"/>
-      <c r="G36" s="8"/>
-      <c r="H36" s="5"/>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A37" s="5"/>
-      <c r="B37" s="5"/>
-      <c r="C37" s="5"/>
-      <c r="D37" s="5"/>
-      <c r="E37" s="6"/>
-      <c r="F37" s="6"/>
-      <c r="G37" s="8"/>
-      <c r="H37" s="5"/>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A38" s="5"/>
-      <c r="B38" s="5"/>
-      <c r="C38" s="5"/>
-      <c r="D38" s="5"/>
-      <c r="E38" s="6"/>
-      <c r="F38" s="6"/>
-      <c r="G38" s="8"/>
-      <c r="H38" s="5"/>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A39" s="5"/>
-      <c r="B39" s="5"/>
-      <c r="C39" s="5"/>
-      <c r="D39" s="5"/>
-      <c r="E39" s="6"/>
-      <c r="F39" s="6"/>
-      <c r="G39" s="8"/>
-      <c r="H39" s="5"/>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A40" s="5"/>
-      <c r="B40" s="5"/>
-      <c r="C40" s="5"/>
-      <c r="D40" s="5"/>
-      <c r="E40" s="6"/>
-      <c r="F40" s="6"/>
-      <c r="G40" s="8"/>
-      <c r="H40" s="5"/>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A41" s="5"/>
-      <c r="B41" s="5"/>
-      <c r="C41" s="5"/>
-      <c r="D41" s="5"/>
-      <c r="E41" s="6"/>
-      <c r="F41" s="6"/>
-      <c r="G41" s="8"/>
-      <c r="H41" s="5"/>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A42" s="5"/>
-      <c r="B42" s="5"/>
-      <c r="C42" s="5"/>
-      <c r="D42" s="5"/>
-      <c r="E42" s="6"/>
-      <c r="F42" s="6"/>
-      <c r="G42" s="8"/>
-      <c r="H42" s="5"/>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A43" s="5"/>
-      <c r="B43" s="5"/>
-      <c r="C43" s="5"/>
-      <c r="D43" s="5"/>
-      <c r="E43" s="6"/>
-      <c r="F43" s="6"/>
-      <c r="G43" s="8"/>
-      <c r="H43" s="5"/>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A44" s="5"/>
-      <c r="B44" s="5"/>
-      <c r="C44" s="5"/>
-      <c r="D44" s="5"/>
-      <c r="E44" s="6"/>
-      <c r="F44" s="6"/>
-      <c r="G44" s="8"/>
-      <c r="H44" s="5"/>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A45" s="5"/>
-      <c r="B45" s="5"/>
-      <c r="C45" s="5"/>
-      <c r="D45" s="5"/>
-      <c r="E45" s="6"/>
-      <c r="F45" s="6"/>
-      <c r="G45" s="8"/>
-      <c r="H45" s="5"/>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A46" s="5"/>
-      <c r="B46" s="5"/>
-      <c r="C46" s="5"/>
-      <c r="D46" s="5"/>
-      <c r="E46" s="6"/>
-      <c r="F46" s="6"/>
-      <c r="G46" s="8"/>
-      <c r="H46" s="5"/>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A47" s="5"/>
-      <c r="B47" s="5"/>
-      <c r="C47" s="5"/>
-      <c r="D47" s="5"/>
-      <c r="E47" s="6"/>
-      <c r="F47" s="6"/>
-      <c r="G47" s="8"/>
-      <c r="H47" s="5"/>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A48" s="5"/>
-      <c r="B48" s="5"/>
-      <c r="C48" s="5"/>
-      <c r="D48" s="5"/>
-      <c r="E48" s="6"/>
-      <c r="F48" s="6"/>
-      <c r="G48" s="8"/>
-      <c r="H48" s="5"/>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="E25" s="5"/>
+      <c r="F25" s="5"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="E26" s="5"/>
+      <c r="F26" s="5"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="E27" s="5"/>
+      <c r="F27" s="5"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="E28" s="5"/>
+      <c r="F28" s="5"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="E29" s="5"/>
+      <c r="F29" s="5"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="E30" s="5"/>
+      <c r="F30" s="5"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="E31" s="5"/>
+      <c r="F31" s="5"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="E32" s="5"/>
+      <c r="F32" s="5"/>
+    </row>
+    <row r="33" spans="5:6" x14ac:dyDescent="0.15">
+      <c r="E33" s="5"/>
+      <c r="F33" s="5"/>
+    </row>
+    <row r="34" spans="5:6" x14ac:dyDescent="0.15">
+      <c r="E34" s="5"/>
+      <c r="F34" s="5"/>
+    </row>
+    <row r="35" spans="5:6" x14ac:dyDescent="0.15">
+      <c r="E35" s="5"/>
+      <c r="F35" s="5"/>
+    </row>
+    <row r="36" spans="5:6" x14ac:dyDescent="0.15">
+      <c r="E36" s="5"/>
+      <c r="F36" s="5"/>
+    </row>
+    <row r="37" spans="5:6" x14ac:dyDescent="0.15">
+      <c r="E37" s="5"/>
+      <c r="F37" s="5"/>
+    </row>
+    <row r="38" spans="5:6" x14ac:dyDescent="0.15">
+      <c r="E38" s="5"/>
+      <c r="F38" s="5"/>
+    </row>
+    <row r="39" spans="5:6" x14ac:dyDescent="0.15">
+      <c r="E39" s="5"/>
+      <c r="F39" s="5"/>
+    </row>
+    <row r="40" spans="5:6" x14ac:dyDescent="0.15">
+      <c r="E40" s="5"/>
+      <c r="F40" s="5"/>
+    </row>
+    <row r="41" spans="5:6" x14ac:dyDescent="0.15">
+      <c r="E41" s="5"/>
+      <c r="F41" s="5"/>
+    </row>
+    <row r="42" spans="5:6" x14ac:dyDescent="0.15">
+      <c r="E42" s="5"/>
+      <c r="F42" s="5"/>
+    </row>
+    <row r="43" spans="5:6" x14ac:dyDescent="0.15">
+      <c r="E43" s="5"/>
+      <c r="F43" s="5"/>
+    </row>
+    <row r="44" spans="5:6" x14ac:dyDescent="0.15">
+      <c r="E44" s="5"/>
+      <c r="F44" s="5"/>
+    </row>
+    <row r="45" spans="5:6" x14ac:dyDescent="0.15">
+      <c r="E45" s="5"/>
+      <c r="F45" s="5"/>
+    </row>
+    <row r="46" spans="5:6" x14ac:dyDescent="0.15">
+      <c r="E46" s="5"/>
+      <c r="F46" s="5"/>
+    </row>
+    <row r="47" spans="5:6" x14ac:dyDescent="0.15">
+      <c r="E47" s="5"/>
+      <c r="F47" s="5"/>
+    </row>
+    <row r="48" spans="5:6" x14ac:dyDescent="0.15">
+      <c r="E48" s="5"/>
+      <c r="F48" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1579,7 +1411,7 @@
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" scale="62" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="88" orientation="landscape" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
   <colBreaks count="1" manualBreakCount="1">
     <brk id="8" max="1048575" man="1"/>

</xml_diff>